<commit_message>
subgroup and moderation analyses
</commit_message>
<xml_diff>
--- a/dataTest.xlsx
+++ b/dataTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivanropovik/Library/Mobile Documents/com~apple~CloudDocs/MANUSCRIPTS/submitted/2017 Meta-Analysis Social Thermoregulation/social-thermoregulation-meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CCD755-96EC-4848-903D-C0E5C57B272B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1112EE-CD6A-4E4E-9E0B-5BAEFBC5439A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16900" xr2:uid="{FBB1F03B-7264-BD4C-8A22-A332DBA6FD1E}"/>
   </bookViews>
@@ -1989,8 +1989,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC35EA7-A2BF-3841-A4A6-D6AF7FF12BBE}">
   <dimension ref="A1:FB348"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="V1" sqref="V1"/>
+      <selection pane="bottomLeft" activeCell="AE234" sqref="AE234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>